<commit_message>
Scalability Update + File System
</commit_message>
<xml_diff>
--- a/Documents/CIFS_commands.xlsx
+++ b/Documents/CIFS_commands.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="37680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="37680" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Create" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,18 +18,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -43,7 +35,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -51,30 +43,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -440,123 +414,103 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V3"/>
+  <dimension ref="A1:R3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>local_path</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>continue_available_enabled</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>oplock_enabled</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>nofiy_enabled</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>file_system_id</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>notify_enabled</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>offline_file_mode</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>ip_control_enabled</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>audit_items</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>share_type</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>file_filter_enable</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>abe_enabled</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>apply_default_acl</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>show_previous_versions_enabled</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>show_snapshot_enabled</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>browse_enabled</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
         <is>
           <t>file_system_name</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>offline_file_mode</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>smb2_ca_enable</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>ip_control_enabled</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>abe_enabled</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>audit_items</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>file_filter_enable</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>apply_default_acl</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>share_type</t>
-        </is>
-      </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>show_previous_versions_enabled</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
-        <is>
-          <t>show_snapshot_enabled</t>
-        </is>
-      </c>
-      <c r="R1" s="1" t="inlineStr">
-        <is>
-          <t>browse_enable</t>
-        </is>
-      </c>
-      <c r="S1" s="1" t="inlineStr">
-        <is>
-          <t>readdir_timeout</t>
-        </is>
-      </c>
-      <c r="T1" s="1" t="inlineStr">
-        <is>
-          <t>lease_enable</t>
-        </is>
-      </c>
-      <c r="U1" s="1" t="inlineStr">
-        <is>
-          <t>dir_unmask</t>
-        </is>
-      </c>
-      <c r="V1" s="1" t="inlineStr">
-        <is>
-          <t>file_unmask</t>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>lease_enabled</t>
+        </is>
+      </c>
+      <c r="Q1" t="inlineStr">
+        <is>
+          <t>dir_umask</t>
+        </is>
+      </c>
+      <c r="R1" t="inlineStr">
+        <is>
+          <t>file_umask</t>
         </is>
       </c>
     </row>
@@ -576,11 +530,6 @@
           <t>yes</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -593,19 +542,23 @@
           <t>path2</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>yes</t>
-        </is>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>no</t>
-        </is>
-      </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <dataValidations count="4">
+    <dataValidation sqref="C2:D1048576 F2:F1048576 I2:N1048576 P2:P1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." type="list">
+      <formula1>"yes,no"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." type="list">
+      <formula1>"none,manual,documents,programs"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." type="list">
+      <formula1>"all,none,open,create,read,write,close,delete,rename,get_security,set_security,get_attr,set_attr,get_xattr,set_xattr"</formula1>
+    </dataValidation>
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." type="list">
+      <formula1>"normal,homedir"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -615,125 +568,122 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S2"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>share_id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>share_name</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>oplock_enabled</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>continue_available_enabled</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>notify_enabled</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>offline_file_mode</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>smb2_ca_enabled</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>ip_control_enabled</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>audit_items</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>share_type</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>file_filter_enable</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
         <is>
           <t>abe_enabled</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>audit_items</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>file_filter_enable</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>apply_default_acl</t>
         </is>
       </c>
-      <c r="M1" s="1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>show_previous_versions_enabled</t>
         </is>
       </c>
-      <c r="N1" s="1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>show_snapshot_enabled</t>
         </is>
       </c>
-      <c r="O1" s="1" t="inlineStr">
+      <c r="N1" t="inlineStr">
         <is>
           <t>browse_enabled</t>
         </is>
       </c>
-      <c r="P1" s="1" t="inlineStr">
-        <is>
-          <t>readdir_timeout</t>
-        </is>
-      </c>
-      <c r="Q1" s="1" t="inlineStr">
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>file_system_name</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
         <is>
           <t>lease_enabled</t>
         </is>
       </c>
-      <c r="R1" s="1" t="inlineStr">
+      <c r="Q1" t="inlineStr">
         <is>
           <t>dir_umask</t>
         </is>
       </c>
-      <c r="S1" s="1" t="inlineStr">
+      <c r="R1" t="inlineStr">
         <is>
           <t>file_umask</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>share1</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>yes</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <dataValidations count="4">
+    <dataValidation sqref="C2:D1048576 F2:F1048576 I2:N1048576 P2:P1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." type="list">
+      <formula1>"yes,no"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." type="list">
+      <formula1>"none,manual,documents,programs"</formula1>
+    </dataValidation>
+    <dataValidation sqref="G2:G1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." type="list">
+      <formula1>"all,none,open,create,read,write,close,delete,rename,get_security,set_security,get_attr,set_attr,get_xattr,set_xattr"</formula1>
+    </dataValidation>
+    <dataValidation sqref="H2:H1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." type="list">
+      <formula1>"normal,homedir"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -743,64 +693,57 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" t="inlineStr">
         <is>
           <t>share_id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" t="inlineStr">
         <is>
           <t>file_system_id</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>share_type</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>share_name</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>file_system_name</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>share_id_list</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>share_name_list</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>share2</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>no</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <dataValidations count="1">
+    <dataValidation sqref="C2:C1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" errorTitle="Invalid Entry" error="Invalid value. Please select from the dropdown." promptTitle="Select Value" prompt="Please select a value from the dropdown." type="list">
+      <formula1>"normal,homedir"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>